<commit_message>
Disable macroeconomic feedbacks with BDMFL file instead of Scenario_BAU
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BDMFL/Boolean Disable Macroecon Feedback Loops.xlsx
+++ b/InputData/ctrl-settings/BDMFL/Boolean Disable Macroecon Feedback Loops.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\BDMFL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\ctrl-settings\BDMFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281EDCBB-60EF-4E49-A907-37031BDDF37B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDMFL" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,23 +192,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -245,23 +227,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,54 +402,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -496,27 +461,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reenable macroeconomic feedback loops
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BDMFL/Boolean Disable Macroecon Feedback Loops.xlsx
+++ b/InputData/ctrl-settings/BDMFL/Boolean Disable Macroecon Feedback Loops.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\ctrl-settings\BDMFL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-virginia\InputData\ctrl-settings\BDMFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B556A75-5638-415C-AE8C-23853A7AEFAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1"/>
+    <workbookView xWindow="450" yWindow="2940" windowWidth="23940" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,6 +193,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -227,6 +245,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,54 +437,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -461,29 +496,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>